<commit_message>
Update currency year to 2019 dollars
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\web-app\OCCF\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="23955" windowHeight="11325"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="OCCF-DpMOCU" sheetId="4" r:id="rId3"/>
     <sheet name="OCCF-DpSOCU" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
 </workbook>
 </file>
 
@@ -67,27 +72,18 @@
     <t>OCCF Dollars per Small Output Currency Unit</t>
   </si>
   <si>
-    <t>billion 2018 dollars</t>
-  </si>
-  <si>
     <t>2018 dollars</t>
   </si>
   <si>
     <t>See cpi.xlsx</t>
   </si>
   <si>
-    <t>which in this case is "2012 dollars per 2018 dollar."</t>
-  </si>
-  <si>
     <t>2012 dollars are worth more than 2018 dollars, so we need a</t>
   </si>
   <si>
     <t>value less than 1 in this variable.</t>
   </si>
   <si>
-    <t>2018 dollars per 2012 dollar</t>
-  </si>
-  <si>
     <t>This is why we multiply, not divide, by the conversion</t>
   </si>
   <si>
@@ -97,19 +93,28 @@
     <t>Medium Output Currency Unit</t>
   </si>
   <si>
-    <t>million 2018 dollars</t>
-  </si>
-  <si>
     <t>OCCF Dollars per Medium Output Currency Unit</t>
   </si>
   <si>
     <t>Recall, this variable is "dollars per large/medium/small currency output unit"</t>
+  </si>
+  <si>
+    <t>2019 dollars per 2012 dollar</t>
+  </si>
+  <si>
+    <t>which in this case is "2012 dollars per 2019 dollar."</t>
+  </si>
+  <si>
+    <t>million 2019 dollars</t>
+  </si>
+  <si>
+    <t>billion 2019 dollars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,7 +230,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,7 +265,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,146 +476,147 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>0.9143273584567535</v>
+        <v>0.89805481563188172</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -628,23 +634,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3">
         <f>10^9*About!$A$26</f>
-        <v>914327358.45675349</v>
+        <v>898054815.63188171</v>
       </c>
     </row>
   </sheetData>
@@ -661,23 +667,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="8">
         <f>10^6*About!$A$26</f>
-        <v>914327.35845675354</v>
+        <v>898054.81563188171</v>
       </c>
     </row>
   </sheetData>
@@ -694,23 +700,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7">
         <f>1*About!A26</f>
-        <v>0.9143273584567535</v>
+        <v>0.89805481563188172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change currency year to 2020
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\web-app\OCCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E145C7-DA32-48E1-AEFA-9C38A9EDE413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="23955" windowHeight="11325"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,18 @@
     <sheet name="OCCF-DpMOCU" sheetId="4" r:id="rId3"/>
     <sheet name="OCCF-DpSOCU" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -72,15 +84,9 @@
     <t>OCCF Dollars per Small Output Currency Unit</t>
   </si>
   <si>
-    <t>2018 dollars</t>
-  </si>
-  <si>
     <t>See cpi.xlsx</t>
   </si>
   <si>
-    <t>2012 dollars are worth more than 2018 dollars, so we need a</t>
-  </si>
-  <si>
     <t>value less than 1 in this variable.</t>
   </si>
   <si>
@@ -102,19 +108,25 @@
     <t>2019 dollars per 2012 dollar</t>
   </si>
   <si>
-    <t>which in this case is "2012 dollars per 2019 dollar."</t>
-  </si>
-  <si>
-    <t>million 2019 dollars</t>
-  </si>
-  <si>
-    <t>billion 2019 dollars</t>
+    <t>2020 dollars</t>
+  </si>
+  <si>
+    <t>million 2020 dollars</t>
+  </si>
+  <si>
+    <t>billion 2020 dollars</t>
+  </si>
+  <si>
+    <t>which in this case is "2012 dollars per 2020 dollar."</t>
+  </si>
+  <si>
+    <t>2012 dollars are worth more than 2020 dollars, so we need a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -263,6 +275,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -298,6 +327,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -473,150 +519,150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.265625" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.89805481563188172</v>
+        <v>0.88711067149387013</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B31" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B33" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -626,7 +672,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -634,23 +680,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3">
         <f>10^9*About!$A$26</f>
-        <v>898054815.63188171</v>
+        <v>887110671.49387014</v>
       </c>
     </row>
   </sheetData>
@@ -659,7 +705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -667,23 +713,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="8">
         <f>10^6*About!$A$26</f>
-        <v>898054.81563188171</v>
+        <v>887110.67149387009</v>
       </c>
     </row>
   </sheetData>
@@ -692,7 +738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -700,23 +746,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7">
         <f>1*About!A26</f>
-        <v>0.89805481563188172</v>
+        <v>0.88711067149387013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update currency units to 2021 USD
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E145C7-DA32-48E1-AEFA-9C38A9EDE413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB702403-E59A-4547-A48B-836A2090D34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,22 +105,22 @@
     <t>Recall, this variable is "dollars per large/medium/small currency output unit"</t>
   </si>
   <si>
-    <t>2019 dollars per 2012 dollar</t>
-  </si>
-  <si>
-    <t>2020 dollars</t>
-  </si>
-  <si>
-    <t>million 2020 dollars</t>
-  </si>
-  <si>
-    <t>billion 2020 dollars</t>
-  </si>
-  <si>
-    <t>which in this case is "2012 dollars per 2020 dollar."</t>
-  </si>
-  <si>
     <t>2012 dollars are worth more than 2020 dollars, so we need a</t>
+  </si>
+  <si>
+    <t>2021 dollars per 2012 dollar</t>
+  </si>
+  <si>
+    <t>billion 2021 dollars</t>
+  </si>
+  <si>
+    <t>million 2021 dollars</t>
+  </si>
+  <si>
+    <t>2021 dollars</t>
+  </si>
+  <si>
+    <t>which in this case is "2012 dollars per 2021 dollar."</t>
   </si>
 </sst>
 </file>
@@ -170,17 +170,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -200,9 +198,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -240,9 +238,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,26 +273,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -327,26 +308,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -523,7 +487,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +529,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -595,44 +559,44 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.88711067149387013</v>
+        <v>0.84730412960844359</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,12 +606,12 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -686,7 +650,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -694,9 +658,9 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <f>10^9*About!$A$26</f>
-        <v>887110671.49387014</v>
+        <v>847304129.60844362</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +683,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -727,9 +691,9 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <f>10^6*About!$A$26</f>
-        <v>887110.67149387009</v>
+        <v>847304.12960844359</v>
       </c>
     </row>
   </sheetData>
@@ -752,7 +716,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -760,9 +724,9 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2">
         <f>1*About!A26</f>
-        <v>0.88711067149387013</v>
+        <v>0.84730412960844359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update About page on OCCF to report correct currency year in all places
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F621025F-0F2F-4C5C-8B8F-F6A4EA98A9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6FEF58-08A4-48D5-A6A7-14155C535D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -108,19 +108,19 @@
     <t>2012 dollars are worth more than 2020 dollars, so we need a</t>
   </si>
   <si>
-    <t>billion 2021 dollars</t>
-  </si>
-  <si>
-    <t>million 2021 dollars</t>
-  </si>
-  <si>
-    <t>2021 dollars</t>
-  </si>
-  <si>
-    <t>which in this case is "2012 dollars per 2021 dollar."</t>
-  </si>
-  <si>
     <t>2023 dollars per 2012 dollar</t>
+  </si>
+  <si>
+    <t>billion 2023 dollars</t>
+  </si>
+  <si>
+    <t>million 2023 dollars</t>
+  </si>
+  <si>
+    <t>2023 dollars</t>
+  </si>
+  <si>
+    <t>which in this case is "2012 dollars per 2023 dollar."</t>
   </si>
 </sst>
 </file>
@@ -487,30 +487,30 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,113 +518,113 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.75350342301658668</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>19</v>
       </c>
@@ -644,17 +644,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -677,17 +677,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -710,17 +710,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>